<commit_message>
binds recapture and release tables, early and late catch and trap tables
</commit_message>
<xml_diff>
--- a/data-raw/metadata/trap-metadata.xlsx
+++ b/data-raw/metadata/trap-metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/edi-battle-clear-rst/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3884D653-F22D-064C-B71F-9B708C740E0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7097D528-98E8-564B-91D2-6FCC55AD2BBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33840" yWindow="-20360" windowWidth="30240" windowHeight="18880" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="300" yWindow="1420" windowWidth="30240" windowHeight="17360" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="9" r:id="rId1"/>
@@ -246,26 +246,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -648,308 +637,307 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:AMG13"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="19.6640625" style="1"/>
-    <col min="3" max="3" width="17.5" style="1" customWidth="1"/>
+    <col min="1" max="2" width="19.6640625" style="2"/>
+    <col min="3" max="3" width="17.5" style="2" customWidth="1"/>
     <col min="4" max="4" width="13.1640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="5.33203125" style="5" customWidth="1"/>
-    <col min="7" max="7" width="5.6640625" style="5" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="5.33203125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="5.6640625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="12.1640625" style="4" customWidth="1"/>
     <col min="9" max="9" width="14.1640625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="16" style="5" customWidth="1"/>
+    <col min="10" max="10" width="16" style="4" customWidth="1"/>
     <col min="11" max="11" width="17.6640625" style="3" customWidth="1"/>
-    <col min="12" max="13" width="9.1640625" style="5" customWidth="1"/>
-    <col min="14" max="1021" width="19.6640625" style="1"/>
-    <col min="1022" max="1024" width="8.33203125" customWidth="1"/>
+    <col min="12" max="13" width="9.1640625" style="4" customWidth="1"/>
+    <col min="14" max="1021" width="19.6640625" style="2"/>
+    <col min="1022" max="1024" width="8.33203125" style="2" customWidth="1"/>
+    <col min="1025" max="16384" width="19.6640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="34" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="J2" s="4"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="7"/>
-    </row>
-    <row r="3" spans="1:13" ht="34" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="L2" s="5"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="L3" s="8" t="s">
+      <c r="L3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="M3" s="8" t="s">
+      <c r="M3" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="L4" s="8" t="s">
+      <c r="L4" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="M4" s="8" t="s">
+      <c r="M4" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="85" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="119" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="85" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="L8" s="5">
+      <c r="L8" s="4">
         <v>381</v>
       </c>
-      <c r="M8" s="5">
+      <c r="M8" s="4">
         <v>115577</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="L9" s="5">
+      <c r="L9" s="4">
         <v>0</v>
       </c>
-      <c r="M9" s="5">
+      <c r="M9" s="4">
         <v>700000</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="34" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="5" t="s">
+      <c r="G10" s="7"/>
+      <c r="H10" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="L10" s="5">
+      <c r="L10" s="4">
         <v>0</v>
       </c>
-      <c r="M10" s="5">
+      <c r="M10" s="4">
         <v>709829</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="85" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="L11" s="5">
+      <c r="L11" s="4">
         <v>0</v>
       </c>
-      <c r="M11" s="5">
+      <c r="M11" s="4">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="51" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="H12" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="L12" s="5">
+      <c r="L12" s="4">
         <v>0.67267580000000005</v>
       </c>
-      <c r="M12" s="5">
+      <c r="M12" s="4">
         <v>3.2650312000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="H13" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="L13" s="5">
+      <c r="L13" s="4">
         <v>0.93</v>
       </c>
-      <c r="M13" s="5">
+      <c r="M13" s="4">
         <v>5.03</v>
       </c>
     </row>
@@ -986,19 +974,19 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.5" style="4" customWidth="1"/>
-    <col min="2" max="2" width="25.1640625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="14" style="4" customWidth="1"/>
+    <col min="1" max="1" width="20.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
removes dead and cleans up subsample for catch. adds back in subsite and removes start counter for trap. updates metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/trap-metadata.xlsx
+++ b/data-raw/metadata/trap-metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/edi-battle-clear-rst/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB238A23-21AB-0A44-9742-F210D01CB1ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F66D8F1-ECA2-A64A-8440-A7FB01855ACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17460" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="101">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -91,9 +91,6 @@
     <t>trap_fishing</t>
   </si>
   <si>
-    <t>counter</t>
-  </si>
-  <si>
     <t>flow_start_meter</t>
   </si>
   <si>
@@ -121,12 +118,6 @@
     <t>Reading on the flow meter at end</t>
   </si>
   <si>
-    <t>start_counter</t>
-  </si>
-  <si>
-    <t>Reading on the rotation counter at the end of the trap visit</t>
-  </si>
-  <si>
     <t>Water velocity measured at trap</t>
   </si>
   <si>
@@ -256,9 +247,6 @@
     <t>nominal</t>
   </si>
   <si>
-    <t>2023-01-02</t>
-  </si>
-  <si>
     <t>trap</t>
   </si>
   <si>
@@ -329,6 +317,18 @@
   </si>
   <si>
     <t>The condition of the trap on the SampleDate and SampleTime. Levels = c("Trap is fishing normal", NA, "There is a partial block in the cone",  "The cone is not rotating", "There is a total block in the cone",  "Trap condition was not provided")</t>
+  </si>
+  <si>
+    <t>2022-09-30</t>
+  </si>
+  <si>
+    <t>end_counter</t>
+  </si>
+  <si>
+    <t>ubc_site</t>
+  </si>
+  <si>
+    <t>Where the trap was located at time of operation. In Battle Creek there are two locations that are used depending on flow conditions. Levels = c("Upper, "Lower")</t>
   </si>
 </sst>
 </file>
@@ -766,20 +766,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="110" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="182.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="200.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.5" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.1640625" style="2" bestFit="1" customWidth="1"/>
@@ -833,16 +833,16 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="L2" s="3"/>
     </row>
@@ -851,25 +851,25 @@
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="L3" s="4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>76</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -877,77 +877,77 @@
         <v>18</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E5" t="s">
-        <v>37</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="L5" s="4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>76</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -955,42 +955,42 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B8" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="L8" s="1">
         <v>3</v>
@@ -1001,28 +1001,28 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C9" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="L9" s="1">
         <v>0</v>
@@ -1033,28 +1033,28 @@
     </row>
     <row r="10" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E10" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="L10" s="1">
         <v>0</v>
@@ -1065,31 +1065,31 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="L11" s="1">
-        <v>0</v>
+        <v>73</v>
       </c>
       <c r="M11" s="1">
         <v>1196242</v>
@@ -1097,28 +1097,28 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B12" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="L12" s="1">
         <v>5</v>
@@ -1129,28 +1129,28 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B13" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E13" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="L13" s="1">
         <v>2</v>
@@ -1161,28 +1161,28 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B14" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="L14" s="1">
         <v>2</v>
@@ -1193,28 +1193,28 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B15" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E15" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="L15" s="1">
         <v>2</v>
@@ -1225,132 +1225,132 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B16" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C16" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E16" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B17" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C17" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E17" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>98</v>
       </c>
       <c r="B18" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C18" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E18" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="L18" s="1">
         <v>0</v>
       </c>
       <c r="M18" s="1">
-        <v>0</v>
+        <v>1000290</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>69</v>
       </c>
       <c r="C19" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E19" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G19" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H19" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="L19" s="1">
         <v>0</v>
       </c>
       <c r="M19" s="1">
-        <v>1000290</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>72</v>
+        <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E20" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="L20" s="1">
         <v>0</v>
       </c>
       <c r="M20" s="1">
-        <v>52</v>
+        <v>483.45</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
@@ -1358,216 +1358,201 @@
         <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C21" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E21" t="s">
+        <v>35</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E21" t="s">
-        <v>38</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="H21" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="L21" s="1">
         <v>0</v>
       </c>
       <c r="M21" s="1">
-        <v>483.45</v>
+        <v>2564</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>34</v>
+        <v>79</v>
       </c>
       <c r="C22" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E22" t="s">
-        <v>38</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="L22" s="1">
-        <v>0</v>
-      </c>
-      <c r="M22" s="1">
-        <v>2564</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="B23" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C23" t="s">
-        <v>35</v>
+        <v>72</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E23" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B24" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="C24" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E24" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>99</v>
       </c>
       <c r="B25" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="C25" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E25" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B26" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C26" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E26" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B27" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C27" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E27" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B28" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C28" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E28" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B29" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C29" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E29" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B30" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C30" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E30" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B31" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C31" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E31" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
standardizes trap station code to match catch
</commit_message>
<xml_diff>
--- a/data-raw/metadata/trap-metadata.xlsx
+++ b/data-raw/metadata/trap-metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liz/Documents/code/edi-battle-clear-rst/data-raw/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F66D8F1-ECA2-A64A-8440-A7FB01855ACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7125B65-6E12-1E4F-8813-99B105F6AEE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17460" tabRatio="834" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -142,9 +142,6 @@
     <t>YYYY-MM-DD</t>
   </si>
   <si>
-    <t>Code referring to the station where the sample was taken. Levels = c("UBC", "LCC", "UCC")</t>
-  </si>
-  <si>
     <t>ratio</t>
   </si>
   <si>
@@ -329,6 +326,9 @@
   </si>
   <si>
     <t>Where the trap was located at time of operation. In Battle Creek there are two locations that are used depending on flow conditions. Levels = c("Upper, "Lower")</t>
+  </si>
+  <si>
+    <t>Code referring to the station where the sample was taken. Levels = c("upper battle creek", "lower battle creek", "lower clear creek",  "upper clear creek", NA, "power house battle creek")</t>
   </si>
 </sst>
 </file>
@@ -767,7 +767,7 @@
   <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -833,13 +833,13 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" t="s">
         <v>32</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E2" t="s">
         <v>33</v>
@@ -857,7 +857,7 @@
         <v>34</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E3" t="s">
         <v>34</v>
@@ -866,10 +866,10 @@
         <v>37</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -883,7 +883,7 @@
         <v>34</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E4" t="s">
         <v>34</v>
@@ -892,24 +892,24 @@
         <v>36</v>
       </c>
       <c r="L4" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="M4" s="4" t="s">
         <v>85</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C5" t="s">
         <v>34</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E5" t="s">
         <v>34</v>
@@ -918,36 +918,36 @@
         <v>37</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C6" t="s">
         <v>34</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E6" t="s">
         <v>34</v>
       </c>
       <c r="J6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="L6" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="L6" s="4" t="s">
-        <v>82</v>
-      </c>
       <c r="M6" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -955,13 +955,13 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>100</v>
       </c>
       <c r="C7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E7" t="s">
         <v>33</v>
@@ -969,28 +969,28 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E8" t="s">
         <v>35</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L8" s="1">
         <v>3</v>
@@ -1001,28 +1001,28 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E9" t="s">
         <v>35</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L9" s="1">
         <v>0</v>
@@ -1039,22 +1039,22 @@
         <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E10" t="s">
         <v>35</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L10" s="1">
         <v>0</v>
@@ -1071,22 +1071,22 @@
         <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E11" t="s">
         <v>35</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L11" s="1">
         <v>73</v>
@@ -1097,28 +1097,28 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E12" t="s">
         <v>35</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L12" s="1">
         <v>5</v>
@@ -1129,28 +1129,28 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E13" t="s">
         <v>35</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L13" s="1">
         <v>2</v>
@@ -1161,28 +1161,28 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E14" t="s">
         <v>35</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L14" s="1">
         <v>2</v>
@@ -1193,28 +1193,28 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E15" t="s">
         <v>35</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L15" s="1">
         <v>2</v>
@@ -1225,16 +1225,16 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E16" t="s">
         <v>33</v>
@@ -1242,16 +1242,16 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E17" t="s">
         <v>33</v>
@@ -1259,28 +1259,28 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B18" t="s">
         <v>27</v>
       </c>
       <c r="C18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E18" t="s">
         <v>35</v>
       </c>
       <c r="F18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="H18" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L18" s="1">
         <v>0</v>
@@ -1291,28 +1291,28 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E19" t="s">
         <v>35</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L19" s="1">
         <v>0</v>
@@ -1329,22 +1329,22 @@
         <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E20" t="s">
         <v>35</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L20" s="1">
         <v>0</v>
@@ -1361,22 +1361,22 @@
         <v>31</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E21" t="s">
         <v>35</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G21" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="L21" s="1">
         <v>0</v>
@@ -1390,13 +1390,13 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C22" t="s">
         <v>32</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E22" t="s">
         <v>33</v>
@@ -1404,16 +1404,16 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E23" t="s">
         <v>33</v>
@@ -1421,16 +1421,16 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B24" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E24" t="s">
         <v>33</v>
@@ -1438,16 +1438,16 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>98</v>
+      </c>
+      <c r="B25" t="s">
         <v>99</v>
       </c>
-      <c r="B25" t="s">
-        <v>100</v>
-      </c>
       <c r="C25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E25" t="s">
         <v>33</v>
@@ -1455,16 +1455,16 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E26" t="s">
         <v>33</v>
@@ -1472,16 +1472,16 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E27" t="s">
         <v>33</v>
@@ -1489,16 +1489,16 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B28" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E28" t="s">
         <v>33</v>
@@ -1506,16 +1506,16 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E29" t="s">
         <v>33</v>
@@ -1523,16 +1523,16 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C30" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E30" t="s">
         <v>33</v>
@@ -1540,16 +1540,16 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C31" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E31" t="s">
         <v>33</v>

</xml_diff>